<commit_message>
TP1 Grupal, informe en PDF
</commit_message>
<xml_diff>
--- a/TP-1-2015-2C-Alumnos/PlanillaDeMetricas.xlsx
+++ b/TP-1-2015-2C-Alumnos/PlanillaDeMetricas.xlsx
@@ -109,7 +109,7 @@
     <t>Tiempo de Ejecución de Prueba</t>
   </si>
   <si>
-    <t>TP1 - GRUPAL - PRUEBA DE SOFTWARE</t>
+    <t>TP1 - GRUPAL - PRUEBA DE SOFTWARE "Búsqueda numérica"</t>
   </si>
 </sst>
 </file>
@@ -756,11 +756,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -771,61 +778,22 @@
     <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -836,16 +804,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -854,6 +812,48 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1413,29 +1413,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="63"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1461,15 +1461,15 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="82"/>
-      <c r="G3" s="82"/>
-      <c r="H3" s="82"/>
-      <c r="I3" s="82"/>
-      <c r="J3" s="82"/>
-      <c r="K3" s="82"/>
-      <c r="L3" s="82"/>
-      <c r="M3" s="82"/>
-      <c r="N3" s="82"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
@@ -1488,15 +1488,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>3.4722222222222654E-3</v>
       </c>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1520,12 +1520,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="63"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1551,15 +1551,15 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
-      <c r="N7" s="82"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="65"/>
+      <c r="L7" s="65"/>
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
@@ -1578,15 +1578,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>4.7916666666666607E-2</v>
       </c>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="66"/>
+      <c r="J8" s="66"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1610,50 +1610,50 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="62"/>
-      <c r="N10" s="63"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="56"/>
+      <c r="M10" s="56"/>
+      <c r="N10" s="57"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76" t="s">
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="77"/>
-      <c r="H11" s="73" t="s">
+      <c r="G11" s="62"/>
+      <c r="H11" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76" t="s">
+      <c r="I11" s="72"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="77"/>
-      <c r="M11" s="73" t="s">
+      <c r="L11" s="62"/>
+      <c r="M11" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="81" t="s">
+      <c r="N11" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="75"/>
+      <c r="B12" s="78"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1686,8 +1686,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="73"/>
-      <c r="N12" s="81"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="64"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1697,9 +1697,9 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="78"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="79"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="68"/>
       <c r="F13" s="47"/>
       <c r="G13" s="48"/>
       <c r="H13" s="49"/>
@@ -1724,9 +1724,9 @@
         <f t="shared" ref="B14:B16" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="79"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68"/>
       <c r="F14" s="47"/>
       <c r="G14" s="48"/>
       <c r="H14" s="49"/>
@@ -1751,9 +1751,9 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="79"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68"/>
       <c r="F15" s="47"/>
       <c r="G15" s="48"/>
       <c r="H15" s="49"/>
@@ -1778,9 +1778,9 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="79"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
       <c r="F16" s="47"/>
       <c r="G16" s="48"/>
       <c r="H16" s="49"/>
@@ -1801,12 +1801,12 @@
     </row>
     <row r="17" spans="1:16" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="85"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="71"/>
       <c r="F17" s="26">
         <f>SUM(F13:F16)</f>
         <v>0</v>
@@ -1859,12 +1859,12 @@
     </row>
     <row r="19" spans="1:16" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
@@ -1941,33 +1941,33 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="63"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="57"/>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="56" t="s">
+      <c r="B24" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="69">
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="82">
         <f>M17</f>
         <v>0</v>
       </c>
-      <c r="F24" s="70"/>
+      <c r="F24" s="83"/>
       <c r="G24" s="34"/>
       <c r="H24" s="35"/>
       <c r="I24" s="35"/>
@@ -1978,16 +1978,16 @@
       <c r="N24" s="38"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="57"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="71">
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="84">
         <f>IF(M17=0,0,IFERROR(M17/(N17*24),"Error"))</f>
         <v>0</v>
       </c>
-      <c r="F25" s="72"/>
+      <c r="F25" s="85"/>
       <c r="G25" s="36"/>
       <c r="H25" s="37"/>
       <c r="I25" s="37"/>
@@ -1998,16 +1998,16 @@
       <c r="N25" s="39"/>
     </row>
     <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="56" t="s">
+      <c r="B26" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="57"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="69">
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="82">
         <f>IF(K17=0,0,IFERROR(ROUNDUP(K17/(M17/100),0),"Error"))</f>
         <v>0</v>
       </c>
-      <c r="F26" s="70"/>
+      <c r="F26" s="83"/>
       <c r="G26" s="36"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
@@ -2018,16 +2018,16 @@
       <c r="N26" s="39"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="56" t="s">
+      <c r="B27" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="58"/>
-      <c r="E27" s="54">
+      <c r="C27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="74">
         <f>IF(K17=0,0,IFERROR(K17/M17,"Error"))</f>
         <v>0</v>
       </c>
-      <c r="F27" s="55"/>
+      <c r="F27" s="75"/>
       <c r="G27" s="36"/>
       <c r="H27" s="37"/>
       <c r="I27" s="37"/>
@@ -2038,11 +2038,11 @@
       <c r="N27" s="39"/>
     </row>
     <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="57"/>
-      <c r="D28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="60"/>
       <c r="E28" s="43">
         <f>E4</f>
         <v>3.4722222222222654E-3</v>
@@ -2061,11 +2061,11 @@
       <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
       <c r="E29" s="43">
         <f>E8</f>
         <v>4.7916666666666607E-2</v>
@@ -2084,11 +2084,11 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="57"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="60"/>
       <c r="E30" s="43" t="str">
         <f>E21</f>
         <v>Completar</v>
@@ -2107,11 +2107,11 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="57"/>
-      <c r="D31" s="58"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="60"/>
       <c r="E31" s="43">
         <f>L17</f>
         <v>0</v>
@@ -2130,11 +2130,11 @@
       <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="57"/>
-      <c r="D32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="43" t="str">
         <f>J17</f>
         <v>Error</v>
@@ -2153,16 +2153,16 @@
       <c r="N32" s="39"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="66" t="s">
+      <c r="B33" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="67"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="59" t="str">
+      <c r="C33" s="80"/>
+      <c r="D33" s="81"/>
+      <c r="E33" s="76" t="str">
         <f>IF(COUNTIF(E28:E32,"Error")=0,SUM(E28:E32),"Error")</f>
         <v>Error</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="77"/>
       <c r="G33" s="40"/>
       <c r="H33" s="41"/>
       <c r="I33" s="41"/>
@@ -2203,6 +2203,27 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="37">
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="B23:N23"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="C1:N1"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B2:E2"/>
@@ -2219,27 +2240,6 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="F3:N3"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B23:N23"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="H11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>